<commit_message>
Actualización diaria del archivo desde Airtable
</commit_message>
<xml_diff>
--- a/xlsx/file.xlsx
+++ b/xlsx/file.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Entitat</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>Tutoria100</t>
+  </si>
+  <si>
+    <t>Tutoria110</t>
   </si>
 </sst>
 </file>
@@ -1521,7 +1524,84 @@
       <c r="AG10" s="12"/>
       <c r="AH10" s="12"/>
     </row>
-    <row r="11" ht="14.25"/>
+    <row r="11" ht="63.75">
+      <c r="A11" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="9">
+        <v>45606.584502314814</v>
+      </c>
+      <c r="G11" s="9">
+        <v>45621</v>
+      </c>
+      <c r="H11" s="9">
+        <v>45621</v>
+      </c>
+      <c r="I11" s="10">
+        <v>25569.479166666668</v>
+      </c>
+      <c r="J11" s="10">
+        <v>25569.5625</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M11" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N11" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="O11" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="P11" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q11" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="R11" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="S11" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="T11" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="U11" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="V11" s="8"/>
+      <c r="W11" s="12"/>
+      <c r="X11" s="12"/>
+      <c r="Y11" s="12"/>
+      <c r="Z11" s="12"/>
+      <c r="AA11" s="12"/>
+      <c r="AB11" s="12"/>
+      <c r="AC11" s="12"/>
+      <c r="AD11" s="12"/>
+      <c r="AE11" s="12"/>
+      <c r="AF11" s="12"/>
+      <c r="AG11" s="12"/>
+      <c r="AH11" s="12"/>
+    </row>
     <row r="12" ht="14.25"/>
     <row r="13" ht="14.25"/>
     <row r="14" ht="14.25"/>

</xml_diff>